<commit_message>
Refactored the excel behaviour into tags/excel controller
</commit_message>
<xml_diff>
--- a/spec/fixtures/test.xlsx
+++ b/spec/fixtures/test.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="32800" windowHeight="19160"/>
   </bookViews>
   <sheets>
-    <sheet name="NRP" sheetId="1" r:id="rId4"/>
+    <sheet name="NRP" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
   <si>
     <t>July 27, 2015 - August 31, 2015 National Retail Pricing v.2</t>
   </si>
@@ -173,18 +181,23 @@
   </si>
   <si>
     <t>Galaxy J1</t>
+  </si>
+  <si>
+    <t>32GB</t>
+  </si>
+  <si>
+    <t>Blue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="&quot; &quot;&quot;$&quot;* #,##0.00&quot; &quot;;&quot; &quot;&quot;$&quot;* (#,##0.00);&quot; &quot;&quot;$&quot;* &quot;-&quot;??&quot; &quot;"/>
-    <numFmt numFmtId="60" formatCode="&quot;$&quot;#,##0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="&quot; &quot;&quot;$&quot;* #,##0.00&quot; &quot;;&quot; &quot;&quot;$&quot;* \(#,##0.00\);&quot; &quot;&quot;$&quot;* &quot;-&quot;??&quot; &quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -196,18 +209,13 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="18"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
@@ -218,19 +226,19 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="14"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -412,161 +420,208 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="40">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="59" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="59" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="60" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffccffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff7f7f7f"/>
-      <rgbColor rgb="ffc0c0c0"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF7F7F7F"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -758,7 +813,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -767,7 +822,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -776,7 +831,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -785,7 +840,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -794,7 +849,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -803,7 +858,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -915,8 +970,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -924,14 +979,14 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -950,7 +1005,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -958,7 +1013,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -986,7 +1041,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1012,7 +1067,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1038,7 +1093,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1064,7 +1119,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1090,7 +1145,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1116,7 +1171,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1142,7 +1197,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1168,7 +1223,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1194,7 +1249,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1207,9 +1262,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1225,7 +1286,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1244,7 +1305,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1270,7 +1331,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1296,7 +1357,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1322,7 +1383,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1348,7 +1409,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1374,7 +1435,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1400,7 +1461,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1426,7 +1487,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1452,7 +1513,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1478,7 +1539,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1491,9 +1552,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1506,7 +1573,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1525,7 +1592,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1555,7 +1622,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1581,7 +1648,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1607,7 +1674,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1633,7 +1700,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1659,7 +1726,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1685,7 +1752,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1711,7 +1778,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1737,7 +1804,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1763,7 +1830,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1776,23 +1843,32 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C1:D1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.875" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6.875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.25" style="1" customWidth="1"/>
@@ -1801,571 +1877,565 @@
     <col min="5" max="5" width="21.125" style="1" customWidth="1"/>
     <col min="6" max="6" width="6.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.875" style="1" customWidth="1"/>
-    <col min="14" max="256" width="6.875" style="1" customWidth="1"/>
+    <col min="8" max="256" width="6.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.75" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:13" ht="27.75" customHeight="1">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="5"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="3"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" t="s" s="6">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="7">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="7">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="9"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="7"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" t="s" s="10">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="9"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="7"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="12">
+    <row r="4" spans="1:13" ht="15" customHeight="1">
+      <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s" s="12">
+      <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s" s="13">
+      <c r="C4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s" s="14">
+      <c r="D4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s" s="14">
+      <c r="E4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="9"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="7"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="17">
+    <row r="5" spans="1:13" ht="15" customHeight="1">
+      <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s" s="17">
+      <c r="B5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s" s="18">
+      <c r="C5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s" s="19">
+      <c r="D5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s" s="19">
+      <c r="E5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="9"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="7"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="17">
+    <row r="6" spans="1:13" ht="15" customHeight="1">
+      <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s" s="17">
+      <c r="B6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s" s="18">
+      <c r="C6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s" s="19">
+      <c r="D6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s" s="19">
+      <c r="E6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="7"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="17">
+    <row r="7" spans="1:13" ht="15" customHeight="1">
+      <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s" s="17">
+      <c r="B7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s" s="18">
+      <c r="C7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s" s="19">
+      <c r="D7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E7" t="s" s="19">
+      <c r="E7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="9"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="7"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="17">
+    <row r="8" spans="1:13" ht="15" customHeight="1">
+      <c r="A8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s" s="17">
+      <c r="B8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s" s="18">
+      <c r="C8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="F8" s="15"/>
-      <c r="G8" t="s" s="20">
+      <c r="D8" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="9"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="7"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="17">
+    <row r="9" spans="1:13" ht="15" customHeight="1">
+      <c r="A9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s" s="17">
+      <c r="B9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s" s="18">
+      <c r="C9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="F9" s="15"/>
-      <c r="G9" t="s" s="22">
+      <c r="D9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="9"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="7"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="17">
+    <row r="10" spans="1:13" ht="15" customHeight="1">
+      <c r="A10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s" s="17">
+      <c r="B10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s" s="23">
+      <c r="C10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="9"/>
+      <c r="D10" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="7"/>
     </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" t="s" s="17">
+    <row r="11" spans="1:13" ht="15" customHeight="1">
+      <c r="A11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s" s="17">
+      <c r="B11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C11" t="s" s="23">
+      <c r="C11" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D11" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="9"/>
+      <c r="D11" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="7"/>
     </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="17">
+    <row r="12" spans="1:13" ht="15" customHeight="1">
+      <c r="A12" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s" s="17">
+      <c r="B12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s" s="23">
+      <c r="C12" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D12" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="9"/>
+      <c r="D12" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="7"/>
     </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" t="s" s="17">
+    <row r="13" spans="1:13" ht="15" customHeight="1">
+      <c r="A13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s" s="17">
+      <c r="B13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C13" t="s" s="24">
+      <c r="C13" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D13" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="9"/>
+      <c r="D13" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="7"/>
     </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="A14" t="s" s="17">
+    <row r="14" spans="1:13" ht="15" customHeight="1">
+      <c r="A14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B14" t="s" s="17">
+      <c r="B14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s" s="23">
+      <c r="C14" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D14" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="9"/>
+      <c r="D14" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="7"/>
     </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" t="s" s="17">
+    <row r="15" spans="1:13" ht="15" customHeight="1">
+      <c r="A15" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s" s="17">
+      <c r="B15" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C15" t="s" s="23">
+      <c r="C15" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="E15" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="9"/>
+      <c r="D15" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="7"/>
     </row>
-    <row r="16" ht="15" customHeight="1">
-      <c r="A16" t="s" s="17">
+    <row r="16" spans="1:13" ht="15" customHeight="1">
+      <c r="A16" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B16" t="s" s="17">
+      <c r="B16" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C16" t="s" s="23">
+      <c r="C16" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D16" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="E16" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="9"/>
+      <c r="D16" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="7"/>
     </row>
-    <row r="17" ht="15" customHeight="1">
-      <c r="A17" t="s" s="17">
+    <row r="17" spans="1:13" ht="15" customHeight="1">
+      <c r="A17" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s" s="17">
+      <c r="B17" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C17" t="s" s="23">
+      <c r="C17" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D17" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="E17" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="9"/>
+      <c r="D17" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="7"/>
     </row>
-    <row r="18" ht="15" customHeight="1">
-      <c r="A18" t="s" s="17">
+    <row r="18" spans="1:13" ht="15" customHeight="1">
+      <c r="A18" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B18" t="s" s="17">
+      <c r="B18" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C18" t="s" s="18">
+      <c r="C18" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D18" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="E18" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="27"/>
+      <c r="D18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="23"/>
     </row>
-    <row r="19" ht="15" customHeight="1">
-      <c r="A19" t="s" s="17">
+    <row r="19" spans="1:13" ht="15" customHeight="1">
+      <c r="A19" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B19" t="s" s="17">
+      <c r="B19" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C19" t="s" s="18">
+      <c r="C19" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D19" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="E19" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="27"/>
+      <c r="D19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="23"/>
     </row>
-    <row r="20" ht="15" customHeight="1">
-      <c r="A20" t="s" s="17">
+    <row r="20" spans="1:13" ht="15" customHeight="1">
+      <c r="A20" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B20" t="s" s="17">
+      <c r="B20" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C20" t="s" s="18">
+      <c r="C20" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D20" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="E20" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="30"/>
+      <c r="D20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="24"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="26"/>
     </row>
-    <row r="21" ht="15" customHeight="1">
-      <c r="A21" t="s" s="17">
+    <row r="21" spans="1:13" ht="15" customHeight="1">
+      <c r="A21" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B21" t="s" s="17">
+      <c r="B21" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C21" t="s" s="18">
+      <c r="C21" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D21" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="E21" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="F21" s="15"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="9"/>
+      <c r="D21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="11"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="7"/>
     </row>
-    <row r="22" ht="15" customHeight="1">
-      <c r="A22" t="s" s="31">
+    <row r="22" spans="1:13" ht="15" customHeight="1">
+      <c r="A22" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B22" t="s" s="31">
+      <c r="B22" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C22" t="s" s="32">
+      <c r="C22" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="D22" t="s" s="33">
-        <v>21</v>
-      </c>
-      <c r="E22" t="s" s="33">
-        <v>21</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="9"/>
+      <c r="D22" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="7"/>
     </row>
-    <row r="23" ht="15" customHeight="1" hidden="1">
-      <c r="A23" t="s" s="34">
+    <row r="23" spans="1:13" ht="15" hidden="1" customHeight="1">
+      <c r="A23" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" t="s" s="36">
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="37"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="39"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2373,9 +2443,14 @@
     <mergeCell ref="A3:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="40" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageSetup scale="40" orientation="landscape"/>
   <headerFooter>
     <oddFooter>VZW confidential and proprietary information for authorized VZW personnel and  third parties only. Use, disclosure or distribution of this information is strictly prohibited to any unauthorized persons or third parties without written approval from VZW.</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>